<commit_message>
textures and maze edits
Floor prefab in maze
added several textures for maze
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Scrum.xlsx
+++ b/Documentation/Scrum/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\src\SEP4\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E810B84E-B270-4AD9-976B-33DFBCDFDD74}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650529E4-B014-414A-8D99-2945BFA693FE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -81,15 +81,9 @@
     <t>Critical</t>
   </si>
   <si>
-    <t>As deevelopers we want game to contain proceduraly generated mazes</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Game should have smooth animation to change scenes</t>
-  </si>
-  <si>
     <t>Proceduraly generated mazes</t>
   </si>
   <si>
@@ -111,17 +105,98 @@
     <t>Finish maze generation</t>
   </si>
   <si>
-    <t>Users character should see game from first person view</t>
-  </si>
-  <si>
     <t>First person view</t>
+  </si>
+  <si>
+    <t>As a owner I want the game to contain memory training exercise</t>
+  </si>
+  <si>
+    <t>As owner I want the game to contain proceduraly generated mazes</t>
+  </si>
+  <si>
+    <t>As owenr I want the game to have smooth animation to change scenes</t>
+  </si>
+  <si>
+    <t>As owner I want the game to be played from first person view</t>
+  </si>
+  <si>
+    <t>As a owner I want the game to coontain sound effects</t>
+  </si>
+  <si>
+    <t>As owenr I want the game to have menu</t>
+  </si>
+  <si>
+    <t>As owner I want the game to run on both pc and mobile</t>
+  </si>
+  <si>
+    <t>As owner I want the game to be optimized</t>
+  </si>
+  <si>
+    <t>As owner I want multiple levels</t>
+  </si>
+  <si>
+    <t>As owner I want the game to have nice skybox</t>
+  </si>
+  <si>
+    <t>As owner I want to have proccess report</t>
+  </si>
+  <si>
+    <t>As owner I want requirements</t>
+  </si>
+  <si>
+    <t>As owner I want group contract</t>
+  </si>
+  <si>
+    <t>As owner I want personal reflections</t>
+  </si>
+  <si>
+    <t>As owner I want project report</t>
+  </si>
+  <si>
+    <t>As owner I want the game to be controlled via on screen buttons on mobile devices</t>
+  </si>
+  <si>
+    <t>Memory training</t>
+  </si>
+  <si>
+    <t>Sound effects</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Mobile and PC</t>
+  </si>
+  <si>
+    <t>Optimized</t>
+  </si>
+  <si>
+    <t>Multiple levels</t>
+  </si>
+  <si>
+    <t>Skybox</t>
+  </si>
+  <si>
+    <t>Proccess report</t>
+  </si>
+  <si>
+    <t>Project report</t>
+  </si>
+  <si>
+    <t>Mobile controlls</t>
+  </si>
+  <si>
+    <t>Group contract</t>
+  </si>
+  <si>
+    <t>Kajul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +229,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +254,11 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -199,10 +286,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -213,8 +301,10 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,25 +475,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,25 +573,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>9</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.7142857142857144</c:v>
+                  <c:v>83.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4285714285714288</c:v>
+                  <c:v>69.285714285714278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1428571428571432</c:v>
+                  <c:v>55.428571428571416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8571428571428577</c:v>
+                  <c:v>41.571428571428555</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5714285714285721</c:v>
+                  <c:v>27.714285714285698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2857142857142863</c:v>
+                  <c:v>13.85714285714284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,7 +1683,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,14 +1731,14 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5">
         <f>'Project Backloog'!C3</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1657,12 +1747,12 @@
       <c r="H2" s="6"/>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I14" si="0">SUM(C2:H2)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5">
         <f>'Project Backloog'!C4</f>
@@ -1681,11 +1771,11 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5">
         <f>'Project Backloog'!C5</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1699,8 +1789,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5">
+        <f>'Project Backloog'!C6</f>
+        <v>30</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1713,8 +1808,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5">
+        <f>'Project Backloog'!C7</f>
+        <v>5</v>
+      </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1727,8 +1827,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5">
+        <f>'Project Backloog'!C8</f>
+        <v>2</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1741,8 +1846,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5">
+        <f>'Project Backloog'!C9</f>
+        <v>2</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1755,8 +1865,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="5">
+        <f>'Project Backloog'!C10</f>
+        <v>8</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1769,8 +1884,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="5">
+        <f>'Project Backloog'!C11</f>
+        <v>20</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1783,8 +1903,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5">
+        <f>'Project Backloog'!C12</f>
+        <v>2</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1797,9 +1922,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5">
+        <f>'Project Backloog'!C13</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1807,12 +1939,17 @@
       <c r="H12" s="6"/>
       <c r="I12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="5">
+        <f>'Project Backloog'!C17</f>
+        <v>1</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1825,8 +1962,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5">
+        <f>'Project Backloog'!C18</f>
+        <v>10</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1847,31 +1989,31 @@
       </c>
       <c r="B16" s="5">
         <f>SUM(B2:B14)</f>
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C16" s="5">
         <f>B16-(SUM(C2:C14))</f>
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" ref="D16:H16" si="1">C16-(SUM(D2:D14))</f>
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1880,31 +2022,31 @@
       </c>
       <c r="B17" s="5">
         <f>SUM(B2:B14)</f>
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C17" s="7">
         <f>B17-($B$17/7)</f>
-        <v>7.7142857142857144</v>
+        <v>83.142857142857139</v>
       </c>
       <c r="D17" s="7">
         <f t="shared" ref="D17:H17" si="2">C17-($B$17/7)</f>
-        <v>6.4285714285714288</v>
+        <v>69.285714285714278</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="2"/>
-        <v>5.1428571428571432</v>
+        <v>55.428571428571416</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>3.8571428571428577</v>
+        <v>41.571428571428555</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" si="2"/>
-        <v>2.5714285714285721</v>
+        <v>27.714285714285698</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="2"/>
-        <v>1.2857142857142863</v>
+        <v>13.85714285714284</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1918,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,17 +2087,17 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="C3" s="10">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,13 +2105,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,10 +2122,278 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C14:C16)</f>
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11.1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>11.2</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11.3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1996,15 +2406,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
@@ -2040,16 +2451,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2060,16 +2471,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2080,16 +2491,36 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11.2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2576,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F10"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Level 01 maze done
Statues imported
Exit temple imported and designed
Scrum files updated
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Scrum.xlsx
+++ b/Documentation/Scrum/Scrum.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\src\SEP4\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650529E4-B014-414A-8D99-2945BFA693FE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC63F2-20D3-4802-8662-5F1F13CC6DF6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Project Backloog" sheetId="2" r:id="rId2"/>
     <sheet name="19.04" sheetId="4" r:id="rId3"/>
-    <sheet name="24.04" sheetId="7" r:id="rId4"/>
-    <sheet name="26.04" sheetId="9" r:id="rId5"/>
+    <sheet name="22.04" sheetId="7" r:id="rId4"/>
+    <sheet name="25.04" sheetId="9" r:id="rId5"/>
     <sheet name="28.04" sheetId="10" r:id="rId6"/>
     <sheet name="01.05" sheetId="11" r:id="rId7"/>
     <sheet name="03.05" sheetId="12" r:id="rId8"/>
@@ -26,8 +26,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'01.05'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'03.05'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'19.04'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'24.04'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'26.04'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'22.04'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'25.04'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'28.04'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -90,21 +90,12 @@
     <t>Fade in and fade our animations</t>
   </si>
   <si>
-    <t>Create algorithm for maze generation</t>
-  </si>
-  <si>
     <t>Marek</t>
   </si>
   <si>
     <t>Done</t>
   </si>
   <si>
-    <t>Implement creating walls and floors</t>
-  </si>
-  <si>
-    <t>Finish maze generation</t>
-  </si>
-  <si>
     <t>First person view</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>As owner I want the game to be played from first person view</t>
   </si>
   <si>
-    <t>As a owner I want the game to coontain sound effects</t>
-  </si>
-  <si>
     <t>As owenr I want the game to have menu</t>
   </si>
   <si>
@@ -144,12 +132,6 @@
     <t>As owner I want requirements</t>
   </si>
   <si>
-    <t>As owner I want group contract</t>
-  </si>
-  <si>
-    <t>As owner I want personal reflections</t>
-  </si>
-  <si>
     <t>As owner I want project report</t>
   </si>
   <si>
@@ -190,6 +172,117 @@
   </si>
   <si>
     <t>Kajul</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>As owner I want the maze to look nice</t>
+  </si>
+  <si>
+    <t>Maze textures</t>
+  </si>
+  <si>
+    <t>Find algorythm for maze genration</t>
+  </si>
+  <si>
+    <t>Implement algorythm in project</t>
+  </si>
+  <si>
+    <t>Test maze generation</t>
+  </si>
+  <si>
+    <t>Find nice bush textures</t>
+  </si>
+  <si>
+    <t>As owner I want the maze to contain statues, which will lead to mini games</t>
+  </si>
+  <si>
+    <t>Statues</t>
+  </si>
+  <si>
+    <t>Write requirements</t>
+  </si>
+  <si>
+    <t>As a owner I want the game to contain sound effects</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>As owner I want nice background music</t>
+  </si>
+  <si>
+    <t>Background music</t>
+  </si>
+  <si>
+    <t>As owner I want project description</t>
+  </si>
+  <si>
+    <t>As owner I want project initiation</t>
+  </si>
+  <si>
+    <t>As owner I want project execution</t>
+  </si>
+  <si>
+    <t>As owner I want group policy</t>
+  </si>
+  <si>
+    <t>As owner I want group description</t>
+  </si>
+  <si>
+    <t>As owner I want abstract</t>
+  </si>
+  <si>
+    <t>As owner I want Introduction</t>
+  </si>
+  <si>
+    <t>As owner I want analysis</t>
+  </si>
+  <si>
+    <t>As owner I want design documentation</t>
+  </si>
+  <si>
+    <t>As owner I want implementation documentation</t>
+  </si>
+  <si>
+    <t>As owner I want test documentation</t>
+  </si>
+  <si>
+    <t>As owner I want project future</t>
+  </si>
+  <si>
+    <t>As owner I want conclusion and results</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Find nice pavement textures</t>
+  </si>
+  <si>
+    <t>Write introduction</t>
+  </si>
+  <si>
+    <t>Find statues on asset store</t>
+  </si>
+  <si>
+    <t>Import statues into scenes</t>
+  </si>
+  <si>
+    <t>Find nice skybox</t>
+  </si>
+  <si>
+    <t>As owner I want I want nice labyrinth exit in the center</t>
+  </si>
+  <si>
+    <t>Labyrinth exit</t>
+  </si>
+  <si>
+    <t>Find nice assets for labyrinth exit</t>
+  </si>
+  <si>
+    <t>Design nice looking exit with lights and particles</t>
   </si>
 </sst>
 </file>
@@ -290,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -302,6 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -412,7 +506,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$16</c:f>
+              <c:f>'Burndown Chart'!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -470,30 +564,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$16:$H$16</c:f>
+              <c:f>'Burndown Chart'!$B$23:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>97</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92</c:v>
+                  <c:v>141.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -510,7 +604,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$17</c:f>
+              <c:f>'Burndown Chart'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -568,30 +662,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$17:$H$17</c:f>
+              <c:f>'Burndown Chart'!$B$24:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>97</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.142857142857139</c:v>
+                  <c:v>126.85714285714286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.285714285714278</c:v>
+                  <c:v>105.71428571428572</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.428571428571416</c:v>
+                  <c:v>84.571428571428584</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.571428571428555</c:v>
+                  <c:v>63.428571428571445</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.714285714285698</c:v>
+                  <c:v>42.285714285714306</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.85714285714284</c:v>
+                  <c:v>21.142857142857164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1348,13 +1442,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1680,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,10 +1829,10 @@
       </c>
       <c r="B2" s="5">
         <f>'Project Backloog'!C3</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -1746,8 +1840,8 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="5">
-        <f t="shared" ref="I2:I14" si="0">SUM(C2:H2)</f>
-        <v>4</v>
+        <f t="shared" ref="I2:I20" si="0">SUM(C2:H2)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1771,7 +1865,7 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5">
         <f>'Project Backloog'!C5</f>
@@ -1790,7 +1884,7 @@
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5">
         <f>'Project Backloog'!C6</f>
@@ -1809,7 +1903,7 @@
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="5">
         <f>'Project Backloog'!C7</f>
@@ -1828,7 +1922,7 @@
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5">
         <f>'Project Backloog'!C8</f>
@@ -1847,7 +1941,7 @@
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" s="5">
         <f>'Project Backloog'!C9</f>
@@ -1866,7 +1960,7 @@
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5">
         <f>'Project Backloog'!C10</f>
@@ -1885,7 +1979,7 @@
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B10" s="5">
         <f>'Project Backloog'!C11</f>
@@ -1904,30 +1998,32 @@
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5">
         <f>'Project Backloog'!C12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5">
         <f>'Project Backloog'!C13</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -1944,29 +2040,33 @@
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
-        <f>'Project Backloog'!C17</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+        <f>'Project Backloog'!C19</f>
+        <v>30</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.5</v>
+      </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5">
-        <f>'Project Backloog'!C18</f>
+        <f>'Project Backloog'!C29</f>
         <v>10</v>
       </c>
       <c r="C14" s="6"/>
@@ -1981,76 +2081,203 @@
       </c>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="5">
+        <f>'Project Backloog'!C30</f>
+        <v>7</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="5">
+        <f>'Project Backloog'!C31</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="5">
+        <f>'Project Backloog'!C32</f>
+        <v>2</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B16" s="5">
-        <f>SUM(B2:B14)</f>
-        <v>97</v>
-      </c>
-      <c r="C16" s="5">
-        <f>B16-(SUM(C2:C14))</f>
-        <v>92</v>
-      </c>
-      <c r="D16" s="5">
-        <f t="shared" ref="D16:H16" si="1">C16-(SUM(D2:D14))</f>
-        <v>92</v>
-      </c>
-      <c r="E16" s="5">
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="5">
+        <f>'Project Backloog'!C33</f>
+        <v>3</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="5">
+        <f>'Project Backloog'!C34</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5">
+        <f>'Project Backloog'!C35</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5">
+        <f>SUM(B2:B20)</f>
+        <v>148</v>
+      </c>
+      <c r="C23" s="5">
+        <f>B23-(SUM(C2:C14))</f>
+        <v>141.5</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" ref="D23:H23" si="1">C23-(SUM(D2:D14))</f>
+        <v>138</v>
+      </c>
+      <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="F16" s="5">
+        <v>138</v>
+      </c>
+      <c r="F23" s="5">
         <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="G16" s="5">
+        <v>138</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="H16" s="5">
+        <v>138</v>
+      </c>
+      <c r="H23" s="5">
         <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5">
-        <f>SUM(B2:B14)</f>
-        <v>97</v>
-      </c>
-      <c r="C17" s="7">
-        <f>B17-($B$17/7)</f>
-        <v>83.142857142857139</v>
-      </c>
-      <c r="D17" s="7">
-        <f t="shared" ref="D17:H17" si="2">C17-($B$17/7)</f>
-        <v>69.285714285714278</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="B24" s="5">
+        <f>SUM(B2:B20)</f>
+        <v>148</v>
+      </c>
+      <c r="C24" s="7">
+        <f>B24-($B$24/7)</f>
+        <v>126.85714285714286</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" ref="D24:H24" si="2">C24-($B$24/7)</f>
+        <v>105.71428571428572</v>
+      </c>
+      <c r="E24" s="7">
         <f t="shared" si="2"/>
-        <v>55.428571428571416</v>
-      </c>
-      <c r="F17" s="7">
+        <v>84.571428571428584</v>
+      </c>
+      <c r="F24" s="7">
         <f t="shared" si="2"/>
-        <v>41.571428571428555</v>
-      </c>
-      <c r="G17" s="7">
+        <v>63.428571428571445</v>
+      </c>
+      <c r="G24" s="7">
         <f t="shared" si="2"/>
-        <v>27.714285714285698</v>
-      </c>
-      <c r="H17" s="7">
+        <v>42.285714285714306</v>
+      </c>
+      <c r="H24" s="7">
         <f t="shared" si="2"/>
-        <v>13.85714285714284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:8" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>21.142857142857164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2060,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,10 +2321,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,7 +2352,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2366,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,13 +2374,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,7 +2394,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2181,7 +2408,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,7 +2422,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,21 +2436,21 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2234,39 +2461,39 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f>SUM(C14:C16)</f>
-        <v>4</v>
+        <f>SUM(C14:C18)</f>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="10">
         <v>11.1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="10">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
-        <v>33</v>
+      <c r="D14" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15">
         <v>11.2</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
+      <c r="D15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2280,119 +2507,310 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C20:C28)</f>
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>15</v>
+      <c r="A20" s="10">
+        <v>12.1</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>16</v>
+      <c r="A21" s="10">
+        <v>12.2</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
+      <c r="A22" s="10">
+        <v>12.3</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>18</v>
+        <v>12.4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>19</v>
+        <v>12.5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>20</v>
+        <v>12.6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>21</v>
+        <v>12.7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>22</v>
+        <v>12.8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>23</v>
+        <v>12.9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>25</v>
+      <c r="A30" s="10">
+        <v>14</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="10">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>26</v>
+      <c r="A31" s="10">
+        <v>15</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="10">
+        <v>3</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>17</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="10">
+        <v>3</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>30</v>
       </c>
     </row>
@@ -2406,10 +2824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,16 +2869,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2471,16 +2889,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2491,36 +2909,56 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12.1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2530,15 +2968,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
@@ -2564,6 +3003,186 @@
       </c>
       <c r="F1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>12.3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12.2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>